<commit_message>
added number to index 2
</commit_message>
<xml_diff>
--- a/library/Library_hbrown_11.10.19.xlsx
+++ b/library/Library_hbrown_11.10.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A3E9F9-75FA-3A48-B61B-18F69AC9ACAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B4357-62F1-314B-BF1F-3F71439B9187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>TGAGGTT</t>
   </si>
   <si>
-    <t>SIC_Index_07</t>
-  </si>
-  <si>
     <t>GAGTTGGT</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>Index1_40</t>
+  </si>
+  <si>
+    <t>SIC_Index2_07</t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,19 +792,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="6" t="b">
         <f>FALSE()</f>
@@ -845,19 +845,19 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" s="6" t="b">
         <f>FALSE()</f>
@@ -884,19 +884,19 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="6" t="b">
         <f>FALSE()</f>
@@ -923,19 +923,19 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" s="6" t="b">
         <f>FALSE()</f>
@@ -962,19 +962,19 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" s="6" t="b">
         <f>FALSE()</f>
@@ -1001,19 +1001,19 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="6" t="b">
         <f>FALSE()</f>
@@ -1040,19 +1040,19 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="6" t="b">
         <f>FALSE()</f>
@@ -1079,19 +1079,19 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="6" t="b">
         <f>FALSE()</f>
@@ -1118,19 +1118,19 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" s="6" t="b">
         <f>FALSE()</f>
@@ -1157,19 +1157,19 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11" s="6" t="b">
         <f>FALSE()</f>
@@ -1196,19 +1196,19 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L12" s="6" t="b">
         <f>FALSE()</f>
@@ -1235,19 +1235,19 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L13" s="6" t="b">
         <f>FALSE()</f>
@@ -1274,19 +1274,19 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L14" s="6" t="b">
         <f>FALSE()</f>
@@ -1313,19 +1313,19 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L15" s="6" t="b">
         <f>FALSE()</f>
@@ -1352,19 +1352,19 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L16" s="6" t="b">
         <f>FALSE()</f>
@@ -1391,19 +1391,19 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L17" s="6" t="b">
         <f>FALSE()</f>
@@ -1430,19 +1430,19 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L18" s="6" t="b">
         <f>FALSE()</f>
@@ -1469,19 +1469,19 @@
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L19" s="6" t="b">
         <f>FALSE()</f>
@@ -1508,19 +1508,19 @@
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L20" s="6" t="b">
         <f>FALSE()</f>
@@ -1547,19 +1547,19 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L21" s="6" t="b">
         <f>FALSE()</f>
@@ -1586,19 +1586,19 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L22" s="6" t="b">
         <f>FALSE()</f>
@@ -1625,19 +1625,19 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L23" s="6" t="b">
         <f>FALSE()</f>
@@ -1664,19 +1664,19 @@
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L24" s="6" t="b">
         <f>FALSE()</f>
@@ -1703,19 +1703,19 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L25" s="6" t="b">
         <f>FALSE()</f>
@@ -1742,19 +1742,19 @@
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L26" s="6" t="b">
         <f>FALSE()</f>
@@ -1781,19 +1781,19 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="J27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L27" s="6" t="b">
         <f>FALSE()</f>
@@ -1820,19 +1820,19 @@
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H28" t="s">
-        <v>43</v>
-      </c>
-      <c r="I28" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L28" s="6" t="b">
         <f>FALSE()</f>
@@ -1859,19 +1859,19 @@
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L29" s="6" t="b">
         <f>FALSE()</f>
@@ -1898,19 +1898,19 @@
         <v>29</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s">
-        <v>45</v>
-      </c>
-      <c r="I30" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L30" s="6" t="b">
         <f>FALSE()</f>
@@ -1937,19 +1937,19 @@
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L31" s="6" t="b">
         <f>FALSE()</f>
@@ -1976,19 +1976,19 @@
         <v>31</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L32" s="6" t="b">
         <f>FALSE()</f>
@@ -2015,19 +2015,19 @@
         <v>32</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H33" t="s">
-        <v>48</v>
-      </c>
-      <c r="I33" t="s">
-        <v>15</v>
+        <v>47</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L33" s="6" t="b">
         <f>FALSE()</f>
@@ -2054,19 +2054,19 @@
         <v>33</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L34" s="6" t="b">
         <f>FALSE()</f>
@@ -2093,19 +2093,19 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H35" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" t="s">
-        <v>15</v>
+        <v>49</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L35" s="6" t="b">
         <f>FALSE()</f>
@@ -2132,19 +2132,19 @@
         <v>35</v>
       </c>
       <c r="G36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H36" t="s">
-        <v>51</v>
-      </c>
-      <c r="I36" t="s">
-        <v>15</v>
+        <v>50</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L36" s="6" t="b">
         <f>FALSE()</f>
@@ -2171,19 +2171,19 @@
         <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H37" t="s">
-        <v>52</v>
-      </c>
-      <c r="I37" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L37" s="6" t="b">
         <f>FALSE()</f>
@@ -2210,19 +2210,19 @@
         <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s">
-        <v>53</v>
-      </c>
-      <c r="I38" t="s">
-        <v>15</v>
+        <v>52</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L38" s="6" t="b">
         <f>FALSE()</f>
@@ -2249,19 +2249,19 @@
         <v>38</v>
       </c>
       <c r="G39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H39" t="s">
-        <v>54</v>
-      </c>
-      <c r="I39" t="s">
-        <v>15</v>
+        <v>53</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L39" s="6" t="b">
         <f>FALSE()</f>
@@ -2288,19 +2288,19 @@
         <v>39</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H40" t="s">
-        <v>55</v>
-      </c>
-      <c r="I40" t="s">
-        <v>15</v>
+        <v>54</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L40" s="6" t="b">
         <f>FALSE()</f>
@@ -2327,19 +2327,19 @@
         <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H41" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" t="s">
-        <v>15</v>
+        <v>55</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="J41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L41" s="6" t="b">
         <f>FALSE()</f>

</xml_diff>

<commit_message>
updating files to confrom to standard
</commit_message>
<xml_diff>
--- a/library/Library_hbrown_11.10.19.xlsx
+++ b/library/Library_hbrown_11.10.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B4357-62F1-314B-BF1F-3F71439B9187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C04AA-396A-A04F-AD8C-450458DE6E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,7 +717,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.6640625" customWidth="1"/>
+    <col min="1" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="10" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>